<commit_message>
[task] More timing stuff
</commit_message>
<xml_diff>
--- a/Documentation/Timings.xlsx
+++ b/Documentation/Timings.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brams\eclipse-workspace\ElevatorControlSystem\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C73420-43C2-44CF-B822-5E91090A34C6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81228766-1FA6-43B1-AC2C-BC5A173F4CFB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{12F92FD4-3103-4244-AF99-1DE1D8830C64}"/>
+    <workbookView xWindow="-8790" yWindow="3600" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{12F92FD4-3103-4244-AF99-1DE1D8830C64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId4"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId5"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="9">
   <si>
     <t xml:space="preserve">Arrival Sensors Interface Times (ns): </t>
   </si>
@@ -55,6 +57,12 @@
   </si>
   <si>
     <t>(X_i - X_mean) ^ 2</t>
+  </si>
+  <si>
+    <t>Process Request Times (ns):</t>
+  </si>
+  <si>
+    <t>Open Elevator Door Times (ns):</t>
   </si>
 </sst>
 </file>
@@ -406,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1B8B0E-36D9-44AE-B59E-6A00E9B6BDB3}">
-  <dimension ref="A1:J77"/>
+  <dimension ref="A1:J76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2600,48 +2608,28 @@
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>18393939300</v>
-      </c>
       <c r="J72">
         <v>10017673300</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>32174660600</v>
-      </c>
       <c r="J73">
         <v>47430248100</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>25097481200</v>
-      </c>
       <c r="J74">
         <v>29388767400</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>18077519900</v>
-      </c>
       <c r="J75">
         <v>23115164700</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>27038695100</v>
-      </c>
       <c r="J76">
         <v>20125022100</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>45129987300</v>
       </c>
     </row>
   </sheetData>
@@ -2654,8 +2642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19E18FAB-6E90-497D-BE1D-1DF7052FA373}">
   <dimension ref="A1:E463"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A426" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A463"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10043,11 +10031,568 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D78A2B8-1573-4234-8880-5BDF3D26041B}">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>6465200</v>
+      </c>
+      <c r="B2">
+        <f>AVERAGE(A2:A21)</f>
+        <v>1079815</v>
+      </c>
+      <c r="C2">
+        <f>A2 - $B$2</f>
+        <v>5385385</v>
+      </c>
+      <c r="D2">
+        <f>C2 ^ 2</f>
+        <v>29002371598225</v>
+      </c>
+      <c r="E2">
+        <f xml:space="preserve"> SUM(D2:D21) / 20</f>
+        <v>3133399087275</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>487200</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C21" si="0">A3 - $B$2</f>
+        <v>-592615</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D21" si="1">C3 ^ 2</f>
+        <v>351192538225</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>491000</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>-588815</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>346703104225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>414600</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>-665215</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>442510996225</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>404600</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>-675215</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>455915296225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>339300</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>-740515</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>548362465225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>407100</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>-672715</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>452545471225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1499500</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>419685</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>176135499225</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>271900</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>-807915</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>652726647225</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>351100</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>-728715</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>531025551225</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>6175600</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>5095785</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>25967024766225</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>369400</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>-710415</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>504689472225</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>437200</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>-642615</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>412954038225</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>406000</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>-673815</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>454026654225</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>416800</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>-663015</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>439588890225</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>391000</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>-688815</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>474466104225</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>373900</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>-705915</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>498315987225</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1110100</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>30285</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>917181225</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>468000</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>-611815</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>374317594225</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>316800</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>-763015</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>582191890225</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC8A897-F679-406A-9EAF-081E929A295F}">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1176200</v>
+      </c>
+      <c r="B2">
+        <f>AVERAGE(A2:A17)</f>
+        <v>2396693.75</v>
+      </c>
+      <c r="C2">
+        <f>A2 - $B$2</f>
+        <v>-1220493.75</v>
+      </c>
+      <c r="D2">
+        <f>C2 ^ 2</f>
+        <v>1489604993789.0625</v>
+      </c>
+      <c r="E2">
+        <f xml:space="preserve"> SUM(D2:D17) / 16</f>
+        <v>561520656835.9375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4024600</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C17" si="0">A3 - $B$2</f>
+        <v>1627906.25</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D17" si="1">C3 ^ 2</f>
+        <v>2650078758789.0625</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2654000</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>257306.25</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>66206506289.0625</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2234800</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>-161893.75</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>26209586289.0625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2461100</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>64406.25</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>4148165039.0625</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2477900</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>81206.25</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>6594455039.0625</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1552000</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>-844693.75</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>713507531289.0625</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2463000</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>66306.25</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>4396518789.0625</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2747900</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>351206.25</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>123345830039.0625</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2912000</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>515306.25</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>265540531289.0625</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2330600</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>-66093.75</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>4368383789.0625</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3164600</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>767906.25</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>589680008789.0625</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2471200</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>74506.25</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>5551181289.0625</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2226900</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>-169793.75</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>28829917539.0625</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2750900</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>354206.25</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>125462067539.0625</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>699400</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>-1697293.75</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>2880806073789.0625</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6563199-F3A3-4C92-962B-2AD4BE34B3D4}">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>